<commit_message>
Updating excel with functions
</commit_message>
<xml_diff>
--- a/documents/droppy.xlsx
+++ b/documents/droppy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaviriacc26/Documents/EAFIT/Tópicos Especiales en Ingeniería de Software/Trabajos/Droppy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\corrections\fork\droppy\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{661B1DE1-7134-4648-9F56-D3B97953C4D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B64EE1B8-BE8D-4D90-887A-132194E7BD8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16960" xr2:uid="{D5556A2A-01AF-CF4B-8B29-80FE36B0B119}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D5556A2A-01AF-CF4B-8B29-80FE36B0B119}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>Archivo de Implementación</t>
   </si>
@@ -156,6 +156,33 @@
   </si>
   <si>
     <t>33 -37</t>
+  </si>
+  <si>
+    <t>36-44</t>
+  </si>
+  <si>
+    <t>56-69</t>
+  </si>
+  <si>
+    <t>14-33</t>
+  </si>
+  <si>
+    <t>82-88</t>
+  </si>
+  <si>
+    <t>102-109</t>
+  </si>
+  <si>
+    <t>111-120</t>
+  </si>
+  <si>
+    <t>droppy/app/Http/Controllers/ShoppingCartController.php</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Billetera</t>
   </si>
 </sst>
 </file>
@@ -186,7 +213,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -220,6 +247,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,9 +303,6 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -290,12 +326,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -304,6 +334,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -324,7 +363,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -623,232 +662,260 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A23" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="43.5" customWidth="1"/>
-    <col min="2" max="2" width="49.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="C7" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="C8" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="C9" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+      <c r="C10" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+      <c r="B18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+      <c r="B19" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+      <c r="B21" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>